<commit_message>
Added BOM specifically for Screaming Circuits
</commit_message>
<xml_diff>
--- a/PCB_Designs/DevBoard_PowerMonitor/SC_Files/BoM_SC.xlsx
+++ b/PCB_Designs/DevBoard_PowerMonitor/SC_Files/BoM_SC.xlsx
@@ -1626,8 +1626,8 @@
   </sheetPr>
   <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="D57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,288 +1682,300 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>158</v>
+        <v>112</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>183</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>339</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>288</v>
+        <v>125</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>131</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>289</v>
+        <v>120</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>160</v>
+        <v>195</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>340</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>290</v>
+        <v>113</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>161</v>
+        <v>184</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>341</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>329</v>
+        <v>253</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>162</v>
+        <v>287</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>158</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>106</v>
+        <v>288</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>234</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>358</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>343</v>
+        <v>230</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>305</v>
+        <v>318</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>39</v>
+        <v>289</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>344</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>343</v>
+        <v>340</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>306</v>
+        <v>319</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>54</v>
+        <v>290</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>345</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>343</v>
+        <v>341</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>329</v>
+        <v>342</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>57</v>
+        <v>106</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>347</v>
+        <v>234</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>358</v>
       </c>
       <c r="I11" s="15" t="s">
         <v>343</v>
@@ -1971,25 +1983,28 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>293</v>
+        <v>39</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>239</v>
+        <v>235</v>
+      </c>
+      <c r="H12" s="15" t="s">
+        <v>344</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>343</v>
@@ -1997,83 +2012,86 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>240</v>
+        <v>236</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>345</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>332</v>
+        <v>343</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>94</v>
+        <v>56</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>95</v>
+        <v>58</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>295</v>
+        <v>57</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H15" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>343</v>
@@ -2081,484 +2099,466 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B16">
         <v>1</v>
       </c>
       <c r="C16" t="s">
-        <v>96</v>
+        <v>59</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>350</v>
+        <v>239</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>61</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>297</v>
+        <v>60</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>351</v>
+        <v>240</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="I19" s="15" t="s">
-        <v>329</v>
+        <v>343</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H20" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>329</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>99</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>156</v>
+        <v>299</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G23" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="H23" s="15">
-        <v>1008</v>
+        <v>245</v>
+      </c>
+      <c r="H23" s="15" t="s">
+        <v>352</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>43</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>157</v>
+        <v>300</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G24" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="H24" s="15">
-        <v>1008</v>
+        <v>245</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>352</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>45</v>
+        <v>329</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>101</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="H25" s="15">
-        <v>1008</v>
+        <v>246</v>
+      </c>
+      <c r="H25" s="15" t="s">
+        <v>353</v>
       </c>
       <c r="I25" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>47</v>
+        <v>334</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>156</v>
+        <v>302</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G26" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="H26" s="15">
-        <v>1008</v>
+        <v>247</v>
+      </c>
+      <c r="H26" s="15" t="s">
+        <v>354</v>
       </c>
       <c r="I26" s="15" t="s">
         <v>343</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B27">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>111</v>
+        <v>156</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>357</v>
+        <v>248</v>
+      </c>
+      <c r="H27" s="15">
+        <v>1008</v>
       </c>
       <c r="I27" s="15" t="s">
         <v>343</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>4</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>112</v>
+        <v>157</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="H28" s="16" t="s">
-        <v>357</v>
+        <v>249</v>
+      </c>
+      <c r="H28" s="15">
+        <v>1008</v>
       </c>
       <c r="I28" s="15" t="s">
         <v>343</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>113</v>
+        <v>303</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>357</v>
+        <v>250</v>
+      </c>
+      <c r="H29" s="15">
+        <v>1008</v>
       </c>
       <c r="I29" s="15" t="s">
         <v>343</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>114</v>
+        <v>156</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>357</v>
+        <v>248</v>
+      </c>
+      <c r="H30" s="15">
+        <v>1008</v>
       </c>
       <c r="I30" s="15" t="s">
         <v>343</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="E31" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="G31" s="10" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H31" s="16" t="s">
         <v>357</v>
@@ -2567,30 +2567,30 @@
         <v>343</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>320</v>
       </c>
       <c r="E32" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G32" s="10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H32" s="16" t="s">
         <v>357</v>
@@ -2599,94 +2599,94 @@
         <v>343</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="E33" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="H33" s="17" t="s">
-        <v>358</v>
+        <v>255</v>
+      </c>
+      <c r="H33" s="16" t="s">
+        <v>357</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>343</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="E34" s="10" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="H34" s="17" t="s">
-        <v>358</v>
+        <v>256</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>357</v>
       </c>
       <c r="I34" s="15" t="s">
         <v>343</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>130</v>
+        <v>30</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>312</v>
       </c>
       <c r="E35" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H35" s="17" t="s">
         <v>358</v>
@@ -2695,30 +2695,30 @@
         <v>343</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="E36" s="10" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H36" s="17" t="s">
         <v>358</v>
@@ -2727,30 +2727,30 @@
         <v>343</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>132</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>127</v>
+        <v>31</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>312</v>
+        <v>325</v>
       </c>
       <c r="E37" s="10" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H37" s="17" t="s">
         <v>358</v>
@@ -2759,30 +2759,30 @@
         <v>343</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>4</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H38" s="17" t="s">
         <v>358</v>
@@ -2791,30 +2791,30 @@
         <v>343</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>312</v>
+        <v>320</v>
       </c>
       <c r="E39" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H39" s="17" t="s">
         <v>358</v>
@@ -2823,30 +2823,30 @@
         <v>343</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C40" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>312</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H40" s="17" t="s">
         <v>358</v>
@@ -2855,7 +2855,7 @@
         <v>343</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
@@ -3952,6 +3952,9 @@
       <c r="K80"/>
     </row>
   </sheetData>
+  <sortState ref="A6:L80">
+    <sortCondition ref="A6"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="49" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>